<commit_message>
Worked on script.js. Can now access content and display it partially on site (using DOM). Updated Documentation.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D92E59C-4AF0-274E-B541-E372F4900E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3F3BC2A-50F2-8544-8983-D9571670AD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="460" windowWidth="25040" windowHeight="15540" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added Bootstrap for styling started button styling.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3F3BC2A-50F2-8544-8983-D9571670AD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1620DE0-A5DB-A44C-AC04-9AE784C88471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
+    <workbookView xWindow="3400" yWindow="500" windowWidth="12760" windowHeight="15540" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B63AF-8074-1548-8CD8-04B3B49EF47B}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Worked on Backend script, a little post scrap is now displayed at the correct URL.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1620DE0-A5DB-A44C-AC04-9AE784C88471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A02F069F-E76C-EF45-9731-237634A3318E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="500" windowWidth="12760" windowHeight="15540" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
+    <workbookView xWindow="3400" yWindow="460" windowWidth="17640" windowHeight="15540" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Worked on doc and layout.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A02F069F-E76C-EF45-9731-237634A3318E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{4B2C5821-0646-7444-BAE8-3E4876E6003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="460" windowWidth="17640" windowHeight="15540" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="23420" windowHeight="15540" activeTab="1" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="JSON_1" localSheetId="0">Tabelle1!$A$2:$B$28</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="67">
   <si>
     <t>Index</t>
   </si>
@@ -213,13 +214,52 @@
   </si>
   <si>
     <t>Response for https://www.corona-memory.ch/api/items?per_page=999999&amp;item_set_id=3527</t>
+  </si>
+  <si>
+    <t>o:ingester</t>
+  </si>
+  <si>
+    <t>o:renderer</t>
+  </si>
+  <si>
+    <t>o:item</t>
+  </si>
+  <si>
+    <t>o:source</t>
+  </si>
+  <si>
+    <t>o:media_type</t>
+  </si>
+  <si>
+    <t>o:sha256</t>
+  </si>
+  <si>
+    <t>o:size</t>
+  </si>
+  <si>
+    <t>o:filename</t>
+  </si>
+  <si>
+    <t>o:lang</t>
+  </si>
+  <si>
+    <t>o:original_url</t>
+  </si>
+  <si>
+    <t>o:thumbnail_urls</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Respone for https://www.corona-memory.ch/api/media?item_set_id=3527</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,6 +276,12 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -330,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -346,6 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -666,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B63AF-8074-1548-8CD8-04B3B49EF47B}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,7 +730,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1164,6 +1211,405 @@
       <c r="F30" s="6" t="s">
         <v>8</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3FC8B8-4EBE-FB42-89FD-DEB7B3FAD807}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Worked on conditional buttons.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{C7379D53-4EAF-3649-90F2-35A0CB3194A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D249EB8-62DF-9D4F-8D94-F3308BB2F8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5400" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
   <si>
     <t>Index</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Respone for https://www.corona-memory.ch/api/media?item_set_id=3527</t>
+  </si>
+  <si>
+    <t>Object.values(obj_values[15])[1]</t>
   </si>
 </sst>
 </file>
@@ -714,7 +717,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1222,13 +1225,13 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -1460,7 +1463,9 @@
       <c r="C18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed Button hover problem
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D249EB8-62DF-9D4F-8D94-F3308BB2F8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{C7657C70-DDA8-904C-8709-E85A4EEF608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B63AF-8074-1548-8CD8-04B3B49EF47B}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3FC8B8-4EBE-FB42-89FD-DEB7B3FAD807}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Worked on overall layout, general styling. Chosen a font, and a color theme. Added Entry class in Backend. Added Impressum to footer. Updated toDo. Code Clean Up.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{C7657C70-DDA8-904C-8709-E85A4EEF608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{E90319B2-D55E-8846-B6D1-8927D0E305BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A375F3DA-76A2-A04B-86D5-741029C00B69}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="JSON_1" localSheetId="0">Tabelle1!$A$2:$B$28</definedName>
+    <definedName name="JSON_1" localSheetId="0">Tabelle1!$A$2:$B$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
   <si>
     <t>Index</t>
   </si>
@@ -120,9 +120,6 @@
     <t>o:resource_class</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>o:resource_template</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>maybe</t>
-  </si>
-  <si>
     <t>o:title</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>thumbnail_display_urls</t>
   </si>
   <si>
-    <t>later</t>
-  </si>
-  <si>
     <t>o:created</t>
   </si>
   <si>
@@ -195,12 +186,6 @@
     <t>dcterms:language</t>
   </si>
   <si>
-    <t>bibo:locator</t>
-  </si>
-  <si>
-    <t>yes(language)</t>
-  </si>
-  <si>
     <t>testvoc:location</t>
   </si>
   <si>
@@ -256,6 +241,9 @@
   </si>
   <si>
     <t>Object.values(obj_values[15])[1]</t>
+  </si>
+  <si>
+    <t>dcterms:creator</t>
   </si>
 </sst>
 </file>
@@ -352,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -375,11 +363,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -396,6 +423,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -714,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B63AF-8074-1548-8CD8-04B3B49EF47B}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,7 +766,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -865,8 +901,8 @@
         <v>20</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
+      <c r="F9" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -874,15 +910,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>22</v>
+      <c r="F10" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -890,15 +926,15 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>26</v>
+      <c r="F11" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -906,14 +942,14 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>15</v>
@@ -924,15 +960,15 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>30</v>
+      <c r="F13" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -940,14 +976,14 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>15</v>
@@ -958,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="11" t="s">
@@ -974,15 +1010,15 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>26</v>
+      <c r="F16" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -990,15 +1026,15 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>26</v>
+      <c r="F17" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1006,7 +1042,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="7" t="s">
@@ -1022,15 +1058,15 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>26</v>
+      <c r="F19" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1038,14 +1074,14 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>15</v>
@@ -1056,7 +1092,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="7" t="s">
@@ -1072,7 +1108,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="7" t="s">
@@ -1088,7 +1124,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="7" t="s">
@@ -1104,7 +1140,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="7" t="s">
@@ -1120,7 +1156,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="7" t="s">
@@ -1136,7 +1172,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="7" t="s">
@@ -1152,17 +1188,15 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1170,48 +1204,78 @@
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>26</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="20">
+        <v>27</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>26</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="6" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>28</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>27</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="6" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>29</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1225,7 +1289,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1236,7 +1300,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1342,7 +1406,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1352,10 +1416,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1365,10 +1429,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1378,13 +1442,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4"/>
     </row>
@@ -1393,7 +1457,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>20</v>
@@ -1406,7 +1470,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>20</v>
@@ -1419,7 +1483,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>20</v>
@@ -1432,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>7</v>
@@ -1445,7 +1509,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>7</v>
@@ -1458,13 +1522,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E18" s="4"/>
     </row>
@@ -1473,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>7</v>
@@ -1486,7 +1550,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>7</v>
@@ -1499,7 +1563,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>7</v>
@@ -1512,7 +1576,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>13</v>
@@ -1525,7 +1589,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>7</v>
@@ -1538,10 +1602,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1551,7 +1615,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>7</v>
@@ -1564,7 +1628,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>11</v>
@@ -1577,7 +1641,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>11</v>
@@ -1590,7 +1654,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fixed dates, worked on Omeka ressources templates, fixed video display. Paola Monti still to do.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A04090-BFB3-554F-BE2B-D6FCFE9E3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B67CFB5-87F0-A448-94B1-B859668C3A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="700" windowWidth="24640" windowHeight="15300" xr2:uid="{C5B10FAF-E839-4B42-B123-0982030637A6}"/>
+    <workbookView xWindow="12920" yWindow="0" windowWidth="12680" windowHeight="16000" xr2:uid="{C5B10FAF-E839-4B42-B123-0982030637A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t>Response for https://www.corona-memory.ch/api/items?per_page=999999&amp;item_set_id=3527</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Alternativ key</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -218,13 +215,71 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required by creator </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternativ in template </t>
+  </si>
+  <si>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Beischreibung</t>
+  </si>
+  <si>
+    <t>Geburtsdatum</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Aufenthaltsort</t>
+  </si>
+  <si>
+    <t>Geburtort</t>
+  </si>
+  <si>
+    <t>Zugehörigkeit</t>
+  </si>
+  <si>
+    <t>Sprache</t>
+  </si>
+  <si>
+    <t>Interviewende Person</t>
+  </si>
+  <si>
+    <t>Datum des Interviews</t>
+  </si>
+  <si>
+    <t>Metadata (infos form templates)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,8 +306,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Textkörper)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri (Textkörper)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,8 +387,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF2F92"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -337,11 +429,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -357,6 +595,28 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -365,6 +625,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF2F92"/>
+      <color rgb="FF945F6C"/>
+      <color rgb="FFBFBFBF"/>
       <color rgb="FFFF2600"/>
       <color rgb="FFFF7E79"/>
       <color rgb="FFFF8AD8"/>
@@ -678,439 +941,524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F866C91A-3A29-C449-85C9-472B6A27C343}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="8" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6">
         <v>7</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="9" t="s">
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6">
         <v>10</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6">
         <v>11</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="10" t="s">
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="6">
         <v>12</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="6">
         <v>14</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="11" t="s">
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20">
         <v>15</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="C18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="23">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="6">
         <v>17</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5" t="s">
+      <c r="C20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="6">
         <v>18</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="6">
         <v>19</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="6">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="6">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="12" t="s">
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="6">
         <v>22</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="6">
         <v>23</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="28"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="6">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="6">
         <v>25</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="30">
         <v>26</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="C29" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="16">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="C30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="6">
         <v>28</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="6">
         <v>29</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
-        <v>20</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>22</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>23</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
-        <v>25</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
-        <v>26</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>27</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
-        <v>29</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1131,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1142,10 +1490,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1153,10 +1501,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -1165,10 +1513,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -1177,10 +1525,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -1189,10 +1537,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -1201,10 +1549,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -1213,10 +1561,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -1225,10 +1573,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -1237,10 +1585,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -1249,10 +1597,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>22</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -1261,13 +1609,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1275,10 +1623,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4"/>
     </row>
@@ -1287,10 +1635,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4"/>
     </row>
@@ -1299,10 +1647,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -1311,10 +1659,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -1323,10 +1671,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -1335,13 +1683,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1349,10 +1697,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="4"/>
     </row>
@@ -1361,10 +1709,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -1373,10 +1721,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" s="4"/>
     </row>
@@ -1385,10 +1733,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="4"/>
     </row>
@@ -1397,10 +1745,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="4"/>
     </row>
@@ -1409,10 +1757,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="4"/>
     </row>
@@ -1421,10 +1769,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" s="4"/>
     </row>
@@ -1433,10 +1781,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="4"/>
     </row>
@@ -1445,10 +1793,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="4"/>
     </row>
@@ -1457,10 +1805,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added comments. Updated issues.
</commit_message>
<xml_diff>
--- a/doc/JSON_Response_table.xlsx
+++ b/doc/JSON_Response_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/HistFalk-OralHistoryArchive/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15D9CCB-32B6-6249-B511-D871C390E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87E0FAC-1BEC-FC4C-A7B2-1F7D3D6991BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="460" windowWidth="24640" windowHeight="15300" xr2:uid="{C5B10FAF-E839-4B42-B123-0982030637A6}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="24640" windowHeight="15300" activeTab="1" xr2:uid="{C5B10FAF-E839-4B42-B123-0982030637A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Response for https://www.corona-memory.ch/api/items?per_page=999999&amp;item_set_id=3527</t>
   </si>
@@ -166,15 +166,6 @@
     <t>dcterms:created</t>
   </si>
   <si>
-    <t>testvoc:location</t>
-  </si>
-  <si>
-    <t>cis:startDate</t>
-  </si>
-  <si>
-    <t>o-module-mapping:marker</t>
-  </si>
-  <si>
     <t>Respone for https://www.corona-memory.ch/api/media?item_set_id=3527</t>
   </si>
   <si>
@@ -217,25 +208,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Required by creator </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alternativ in template </t>
   </si>
   <si>
@@ -272,14 +244,14 @@
     <t>Datum des Interviews</t>
   </si>
   <si>
-    <t>Metadata (infos form templates)</t>
+    <t>Metadata (infos form templates, requiered or "ubk")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -307,11 +279,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Textkörper)"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
@@ -326,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,26 +354,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF2F92"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -436,38 +385,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF7030A0"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF7030A0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -501,21 +422,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF7030A0"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -527,21 +433,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF7030A0"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF7030A0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -595,28 +486,20 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -941,524 +824,428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F866C91A-3A29-C449-85C9-472B6A27C343}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="45.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>16</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="27"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="D22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="6">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
         <v>22</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="6">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>24</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>25</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="B28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6">
-        <v>12</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20">
-        <v>15</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="23">
-        <v>16</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="34"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="6">
-        <v>17</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="6">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="6">
-        <v>19</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="6">
-        <v>20</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="B29" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="6">
-        <v>21</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="28"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="6">
-        <v>22</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="6">
-        <v>23</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="6">
-        <v>24</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="28"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="6">
-        <v>25</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="30">
-        <v>26</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="33"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="16">
-        <v>27</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="17"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="6">
-        <v>28</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="6">
-        <v>29</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="4"/>
+      <c r="D29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1469,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF254BB-14C8-BA40-A83D-4F5CA7D406C6}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,7 +1268,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1661,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>6</v>
@@ -1673,7 +1460,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>6</v>
@@ -1685,13 +1472,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1699,7 +1486,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>6</v>
@@ -1711,7 +1498,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>6</v>
@@ -1723,7 +1510,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>6</v>
@@ -1735,7 +1522,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>11</v>
@@ -1747,7 +1534,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>6</v>
@@ -1759,7 +1546,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>21</v>
@@ -1771,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>6</v>
@@ -1783,7 +1570,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>9</v>
@@ -1795,7 +1582,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>9</v>

</xml_diff>